<commit_message>
Updated data api: allowing null values in file upload feature, updated sample files in sails app
</commit_message>
<xml_diff>
--- a/mbtb_app/web_portal/mbtb_portal/assets/files/data_upload_reference.xlsx
+++ b/mbtb_app/web_portal/mbtb_portal/assets/files/data_upload_reference.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niravjadeja/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niravjadeja/Downloads/mbtb-app/mbtb_app/web_portal/mbtb_portal/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D08649-DB1F-974C-8FCE-3D0C54EF4276}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE52A42-10C2-6A49-BDD3-525FF1C13A4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{BCA25266-3726-A341-8F06-DD0F41401FE1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{BCA25266-3726-A341-8F06-DD0F41401FE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>mbtb_code</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>dropdown ('Brain', 'Brain &amp; Spinal', 'Full Body')</t>
+  </si>
+  <si>
+    <t>Only number is allowed, use `null` (without quotes) for empty value.</t>
   </si>
 </sst>
 </file>
@@ -557,7 +560,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,10 +704,10 @@
       <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -733,10 +736,10 @@
       <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">

</xml_diff>